<commit_message>
Made most of the materials. Also implemented simple version structure of the program.
</commit_message>
<xml_diff>
--- a/Material/Työaikaraportti_ArttuMutka.xlsx
+++ b/Material/Työaikaraportti_ArttuMutka.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\School\Ohjelmistokehitys\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\School\Ohjelmistokehitys\Project\Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19497AA5-BB0C-4673-A6A5-FB94F6EAEA93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643420C7-B61D-425C-A646-5A3617DB4F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D29C344C-A0B2-4C12-8324-F197E4D0F762}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11295" xr2:uid="{D29C344C-A0B2-4C12-8324-F197E4D0F762}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Työaikaraportti</t>
   </si>
@@ -51,6 +51,27 @@
   </si>
   <si>
     <t>Yht</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>Laitoin projektin alulle lisäsin tiedostot ja laitoin gitin toimintaan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opetelin ja tein usecase diagrammin ja ideoin ohjelmaa </t>
+  </si>
+  <si>
+    <t>suunitelua, UML diagrammi uudistus uuden suunitelman mukaan ja vaatismääritelyn aloitus</t>
+  </si>
+  <si>
+    <t>Ideoin ominaisuuksia ja miten kirjoitan vaatimusmäärittelyä</t>
+  </si>
+  <si>
+    <t>Ideointia ja kirjoitin vaatimusmäärittelyn</t>
+  </si>
+  <si>
+    <t>Tein ohjelmaa tai no hakkasin päätäni seinään ja olen aika lailla alku pisteessä mutta toivotavasti opin ja pääsen nyt eteenpäin</t>
   </si>
 </sst>
 </file>
@@ -135,11 +156,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -455,15 +480,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A8DA42-B604-4C4D-9F58-45BF577D224E}">
-  <dimension ref="B2:D9"/>
+  <dimension ref="B2:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="63.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="26.25" x14ac:dyDescent="0.4">
@@ -482,30 +509,81 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+    <row r="6" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="B6" s="5">
+        <v>45322</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B9" s="2" t="s">
+      <c r="B7" s="5">
+        <v>45323</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="B8" s="5">
+        <v>45324</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="B9" s="5">
+        <v>45325</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B10" s="5">
+        <v>45326</v>
+      </c>
+      <c r="C10" s="3">
         <v>4</v>
       </c>
-      <c r="C9" s="2">
-        <f>SUM(C6,C8)</f>
-        <v>0</v>
-      </c>
-      <c r="D9" s="2"/>
+      <c r="D10" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="B11" s="5">
+        <v>45327</v>
+      </c>
+      <c r="C11" s="3">
+        <v>8</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="2">
+        <f>SUM(C6:C11)</f>
+        <v>17</v>
+      </c>
+      <c r="D12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Made the navbar be generated dynamically
</commit_message>
<xml_diff>
--- a/Material/Työaikaraportti_ArttuMutka.xlsx
+++ b/Material/Työaikaraportti_ArttuMutka.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\School\Ohjelmistokehitys\Project\Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643420C7-B61D-425C-A646-5A3617DB4F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46714EA2-A630-411F-8C45-06EA6C207BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11295" xr2:uid="{D29C344C-A0B2-4C12-8324-F197E4D0F762}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Työaikaraportti</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Tein ohjelmaa tai no hakkasin päätäni seinään ja olen aika lailla alku pisteessä mutta toivotavasti opin ja pääsen nyt eteenpäin</t>
+  </si>
+  <si>
+    <t>korjasin eilisen virheet ja sain ohjelman perus navigaatio rakenteent toimimaan</t>
   </si>
 </sst>
 </file>
@@ -480,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A8DA42-B604-4C4D-9F58-45BF577D224E}">
-  <dimension ref="B2:D12"/>
+  <dimension ref="B2:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="I13" sqref="I12:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,15 +578,26 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B12" s="2" t="s">
+    <row r="12" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="B12" s="5">
+        <v>45328</v>
+      </c>
+      <c r="C12" s="3">
         <v>4</v>
       </c>
-      <c r="C12" s="2">
-        <f>SUM(C6:C11)</f>
-        <v>17</v>
-      </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="2">
+        <f>SUM(C6:C12)</f>
+        <v>21</v>
+      </c>
+      <c r="D13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added bunch of material. Also made the conversion page and logic
</commit_message>
<xml_diff>
--- a/Material/Työaikaraportti_ArttuMutka.xlsx
+++ b/Material/Työaikaraportti_ArttuMutka.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\School\Ohjelmistokehitys\Project\Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46714EA2-A630-411F-8C45-06EA6C207BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E7160E-C753-4DEB-8619-F1EB4DCA3320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11295" xr2:uid="{D29C344C-A0B2-4C12-8324-F197E4D0F762}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Työaikaraportti</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>korjasin eilisen virheet ja sain ohjelman perus navigaatio rakenteent toimimaan</t>
+  </si>
+  <si>
+    <t>Tein navigaatio palkista dynaamisen ja muutenkin paremman, tein laskimen kokonaisuudessaan ja myöskin yritin oppia ja kehitää vesiputousmallia</t>
+  </si>
+  <si>
+    <t>Aloitin perusrakenteen muunnin sivulle</t>
   </si>
 </sst>
 </file>
@@ -483,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A8DA42-B604-4C4D-9F58-45BF577D224E}">
-  <dimension ref="B2:D13"/>
+  <dimension ref="B2:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I13" sqref="I12:I13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,15 +595,37 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B13" s="2" t="s">
+    <row r="13" spans="2:4" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="B13" s="5">
+        <v>45329</v>
+      </c>
+      <c r="C13" s="3">
+        <v>9</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B14" s="5">
+        <v>45330</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="2">
-        <f>SUM(C6:C12)</f>
-        <v>21</v>
-      </c>
-      <c r="D13" s="2"/>
+      <c r="C15" s="2">
+        <f>SUM(C6:C14)</f>
+        <v>31</v>
+      </c>
+      <c r="D15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added network tools pinger tool and also the cheatsheets page with its functionalities.
</commit_message>
<xml_diff>
--- a/Material/Työaikaraportti_ArttuMutka.xlsx
+++ b/Material/Työaikaraportti_ArttuMutka.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\School\Ohjelmistokehitys\Project\Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E7160E-C753-4DEB-8619-F1EB4DCA3320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321DAD45-15DF-4473-8080-30DA7F54637F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11295" xr2:uid="{D29C344C-A0B2-4C12-8324-F197E4D0F762}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D29C344C-A0B2-4C12-8324-F197E4D0F762}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Työaikaraportti</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>Aloitin perusrakenteen muunnin sivulle</t>
+  </si>
+  <si>
+    <t>Tein logiikan muuntimelle ja parantelin muunnin sivun ulkonäköä.</t>
+  </si>
+  <si>
+    <t>Kehitin verko töykaluihin pinger työkalun ja myöskin kehitin lunttilappu sivun rakenteen ja toiminallisuuden.</t>
   </si>
 </sst>
 </file>
@@ -489,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A8DA42-B604-4C4D-9F58-45BF577D224E}">
-  <dimension ref="B2:D15"/>
+  <dimension ref="B2:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,15 +623,37 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B15" s="2" t="s">
+    <row r="15" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="B15" s="5">
+        <v>45333</v>
+      </c>
+      <c r="C15" s="3">
+        <v>7</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="B16" s="5">
+        <v>45334</v>
+      </c>
+      <c r="C16" s="3">
+        <v>10</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="2">
-        <f>SUM(C6:C14)</f>
-        <v>31</v>
-      </c>
-      <c r="D15" s="2"/>
+      <c r="C17" s="2">
+        <f>SUM(C6:C16)</f>
+        <v>48</v>
+      </c>
+      <c r="D17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Made the navbar have space for the settings and about also wrote the about section.
</commit_message>
<xml_diff>
--- a/Material/Työaikaraportti_ArttuMutka.xlsx
+++ b/Material/Työaikaraportti_ArttuMutka.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\School\Ohjelmistokehitys\Project\Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321DAD45-15DF-4473-8080-30DA7F54637F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06DA63E-F3CD-4222-9747-9FBD9BB37542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D29C344C-A0B2-4C12-8324-F197E4D0F762}"/>
+    <workbookView xWindow="2700" yWindow="2700" windowWidth="21600" windowHeight="11295" xr2:uid="{D29C344C-A0B2-4C12-8324-F197E4D0F762}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Työaikaraportti</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Kehitin verko töykaluihin pinger työkalun ja myöskin kehitin lunttilappu sivun rakenteen ja toiminallisuuden.</t>
+  </si>
+  <si>
+    <t>Koko tämän ajan käytin yritääkseni saamaa lisätyä uusia täppiä navigaatio palkkiin erillään muista. Tämä johti lukemaan dokumentaatiota ja ihmetelemään tekoälyn tyhmiä vastauksia. Lopulta sain todella hyvän lopputuloksen mutta tämä on jo toinen kerta kun navigaatio palkki aiheutti näin paljon pään särkyä saman projektin aikana. Myöskin kirjoitin about sivun.</t>
   </si>
 </sst>
 </file>
@@ -495,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A8DA42-B604-4C4D-9F58-45BF577D224E}">
-  <dimension ref="B2:D17"/>
+  <dimension ref="B2:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,15 +648,31 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B17" s="2" t="s">
+    <row r="17" spans="2:4" ht="131.25" x14ac:dyDescent="0.3">
+      <c r="B17" s="5">
+        <v>45335</v>
+      </c>
+      <c r="C17" s="3">
+        <v>12</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B18" s="5"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="2">
-        <f>SUM(C6:C16)</f>
-        <v>48</v>
-      </c>
-      <c r="D17" s="2"/>
+      <c r="C19" s="2">
+        <f>SUM(C6:C17)</f>
+        <v>60</v>
+      </c>
+      <c r="D19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Made settings for the most part. Made good headway with the stylings just have to continue with them.
</commit_message>
<xml_diff>
--- a/Material/Työaikaraportti_ArttuMutka.xlsx
+++ b/Material/Työaikaraportti_ArttuMutka.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\School\Ohjelmistokehitys\Project\Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06DA63E-F3CD-4222-9747-9FBD9BB37542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE93771-AE22-4036-A3E0-93184FCBCAEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="2700" windowWidth="21600" windowHeight="11295" xr2:uid="{D29C344C-A0B2-4C12-8324-F197E4D0F762}"/>
+    <workbookView xWindow="1425" yWindow="3450" windowWidth="21600" windowHeight="11295" xr2:uid="{D29C344C-A0B2-4C12-8324-F197E4D0F762}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Työaikaraportti</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Koko tämän ajan käytin yritääkseni saamaa lisätyä uusia täppiä navigaatio palkkiin erillään muista. Tämä johti lukemaan dokumentaatiota ja ihmetelemään tekoälyn tyhmiä vastauksia. Lopulta sain todella hyvän lopputuloksen mutta tämä on jo toinen kerta kun navigaatio palkki aiheutti näin paljon pään särkyä saman projektin aikana. Myöskin kirjoitin about sivun.</t>
+  </si>
+  <si>
+    <t>Tein asetukset ja aloin tyylitelemään.</t>
   </si>
 </sst>
 </file>
@@ -501,7 +504,7 @@
   <dimension ref="B2:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,17 +663,23 @@
       </c>
     </row>
     <row r="18" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B18" s="5"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
+      <c r="B18" s="5">
+        <v>45336</v>
+      </c>
+      <c r="C18" s="3">
+        <v>10</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="19" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="2">
-        <f>SUM(C6:C17)</f>
-        <v>60</v>
+        <f>SUM(C6:C18)</f>
+        <v>70</v>
       </c>
       <c r="D19" s="2"/>
     </row>

</xml_diff>

<commit_message>
Improved styles alot. Also fixed bug in calculator with regular characters causing a crash
</commit_message>
<xml_diff>
--- a/Material/Työaikaraportti_ArttuMutka.xlsx
+++ b/Material/Työaikaraportti_ArttuMutka.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\School\Ohjelmistokehitys\Project\Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE93771-AE22-4036-A3E0-93184FCBCAEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64EEDB32-B88E-42C4-A6BA-B4037DF49933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1425" yWindow="3450" windowWidth="21600" windowHeight="11295" xr2:uid="{D29C344C-A0B2-4C12-8324-F197E4D0F762}"/>
+    <workbookView xWindow="-25320" yWindow="315" windowWidth="25440" windowHeight="15270" xr2:uid="{D29C344C-A0B2-4C12-8324-F197E4D0F762}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Työaikaraportti</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Tein asetukset ja aloin tyylitelemään.</t>
+  </si>
+  <si>
+    <t>Tyylitelin ja korjasin bugeja Tyyli alkaa olemaan aika hyvä mutta luulen että kaipaa vielä hiontaa</t>
   </si>
 </sst>
 </file>
@@ -501,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A8DA42-B604-4C4D-9F58-45BF577D224E}">
-  <dimension ref="B2:D19"/>
+  <dimension ref="B2:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,15 +676,26 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B19" s="2" t="s">
+    <row r="19" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="B19" s="5">
+        <v>45337</v>
+      </c>
+      <c r="C19" s="3">
+        <v>7</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="2">
-        <f>SUM(C6:C18)</f>
-        <v>70</v>
-      </c>
-      <c r="D19" s="2"/>
+      <c r="C20" s="2">
+        <f>SUM(C6:C19)</f>
+        <v>77</v>
+      </c>
+      <c r="D20" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Style improvements. also material
</commit_message>
<xml_diff>
--- a/Material/Työaikaraportti_ArttuMutka.xlsx
+++ b/Material/Työaikaraportti_ArttuMutka.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\School\Ohjelmistokehitys\Project\Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64EEDB32-B88E-42C4-A6BA-B4037DF49933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C6E9AD-D16C-4FEB-B9E7-ABFDB603596A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="315" windowWidth="25440" windowHeight="15270" xr2:uid="{D29C344C-A0B2-4C12-8324-F197E4D0F762}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{D29C344C-A0B2-4C12-8324-F197E4D0F762}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Työaikaraportti</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>Tyylitelin ja korjasin bugeja Tyyli alkaa olemaan aika hyvä mutta luulen että kaipaa vielä hiontaa</t>
+  </si>
+  <si>
+    <t>Tyylitelyä lisää alan olemaan kunolla tyytyävinen tyyleihin en täysin implementaatioon saatan perehtyä pystyykö paremapaan.</t>
+  </si>
+  <si>
+    <t>Säädin tyylejä lisää sain ne aika lailla hyviksi.</t>
   </si>
 </sst>
 </file>
@@ -504,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A8DA42-B604-4C4D-9F58-45BF577D224E}">
-  <dimension ref="B2:D20"/>
+  <dimension ref="B2:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,15 +693,37 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B20" s="2" t="s">
+    <row r="20" spans="2:4" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="B20" s="5">
+        <v>45338</v>
+      </c>
+      <c r="C20" s="3">
+        <v>5</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B21" s="5">
+        <v>45339</v>
+      </c>
+      <c r="C21" s="3">
+        <v>3</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="2">
-        <f>SUM(C6:C19)</f>
-        <v>77</v>
-      </c>
-      <c r="D20" s="2"/>
+      <c r="C22" s="2">
+        <f>SUM(C6:C21)</f>
+        <v>85</v>
+      </c>
+      <c r="D22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed a bunch of bugs Calculator - "=" doesnt anymore cause crash when input box empty Cheatsheet - added ability to press enter Cheatsheet - Added proper character handling UTF-8 to enable things like ä Other minor changes
</commit_message>
<xml_diff>
--- a/Material/Työaikaraportti_ArttuMutka.xlsx
+++ b/Material/Työaikaraportti_ArttuMutka.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\School\Ohjelmistokehitys\Project\Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C6E9AD-D16C-4FEB-B9E7-ABFDB603596A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33353248-4329-4F08-B534-5F56EF022EDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{D29C344C-A0B2-4C12-8324-F197E4D0F762}"/>
+    <workbookView xWindow="2595" yWindow="1710" windowWidth="21600" windowHeight="11295" xr2:uid="{D29C344C-A0B2-4C12-8324-F197E4D0F762}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Työaikaraportti</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Säädin tyylejä lisää sain ne aika lailla hyviksi.</t>
+  </si>
+  <si>
+    <t>Tein lievästi tyylien kanssa säätöä. Hankin 3 testaajaa ja sain heiltä ongelmia. Korjasin kyseiset bugit, aloin suunitelemaan ikonia.</t>
   </si>
 </sst>
 </file>
@@ -510,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A8DA42-B604-4C4D-9F58-45BF577D224E}">
-  <dimension ref="B2:D22"/>
+  <dimension ref="B2:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,15 +718,26 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B22" s="2" t="s">
+    <row r="22" spans="2:4" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="B22" s="5">
+        <v>45340</v>
+      </c>
+      <c r="C22" s="3">
+        <v>8</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="2">
-        <f>SUM(C6:C21)</f>
-        <v>85</v>
-      </c>
-      <c r="D22" s="2"/>
+      <c r="C23" s="2">
+        <f>SUM(C6:C22)</f>
+        <v>93</v>
+      </c>
+      <c r="D23" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added the icon to this Also added better functionality to conversion tools.
</commit_message>
<xml_diff>
--- a/Material/Työaikaraportti_ArttuMutka.xlsx
+++ b/Material/Työaikaraportti_ArttuMutka.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\School\Ohjelmistokehitys\Project\Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33353248-4329-4F08-B534-5F56EF022EDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81C5F6A-E7E8-4381-9503-78E597338881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="1710" windowWidth="21600" windowHeight="11295" xr2:uid="{D29C344C-A0B2-4C12-8324-F197E4D0F762}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D29C344C-A0B2-4C12-8324-F197E4D0F762}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Työaikaraportti</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Tein lievästi tyylien kanssa säätöä. Hankin 3 testaajaa ja sain heiltä ongelmia. Korjasin kyseiset bugit, aloin suunitelemaan ikonia.</t>
+  </si>
+  <si>
+    <t>Suunitelin ikonin ja kehitin sen. Tein muunnin työkaluun paranuksia.</t>
   </si>
 </sst>
 </file>
@@ -513,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A8DA42-B604-4C4D-9F58-45BF577D224E}">
-  <dimension ref="B2:D23"/>
+  <dimension ref="B2:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,15 +732,26 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B23" s="2" t="s">
+    <row r="23" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="B23" s="5">
+        <v>45341</v>
+      </c>
+      <c r="C23" s="3">
+        <v>5</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B24" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="2">
-        <f>SUM(C6:C22)</f>
-        <v>93</v>
-      </c>
-      <c r="D23" s="2"/>
+      <c r="C24" s="2">
+        <f>SUM(C6:C23)</f>
+        <v>98</v>
+      </c>
+      <c r="D24" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Made bettter oraganization for pages section, organized tools by their main gategory. Added a checksum tool. Added a random number generator tool. Started making system information.
</commit_message>
<xml_diff>
--- a/Material/Työaikaraportti_ArttuMutka.xlsx
+++ b/Material/Työaikaraportti_ArttuMutka.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\School\Ohjelmistokehitys\Project\Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81C5F6A-E7E8-4381-9503-78E597338881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834FD00C-F600-4505-AD12-6065E5C0A210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D29C344C-A0B2-4C12-8324-F197E4D0F762}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Työaikaraportti</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>Suunitelin ikonin ja kehitin sen. Tein muunnin työkaluun paranuksia.</t>
+  </si>
+  <si>
+    <t>Aloin suunitelemaana lisää ominaisuuksia. Implementoin uusia usercontrol ja niille omat navigaatio osiot. Lajitelin tiedostoja paremmin. Tein random number generaatorin. Tein Yksinkertaisen checksum työkalun</t>
   </si>
 </sst>
 </file>
@@ -516,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A8DA42-B604-4C4D-9F58-45BF577D224E}">
-  <dimension ref="B2:D24"/>
+  <dimension ref="B2:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,15 +746,26 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B24" s="2" t="s">
+    <row r="24" spans="2:4" ht="93.75" x14ac:dyDescent="0.3">
+      <c r="B24" s="5">
+        <v>45345</v>
+      </c>
+      <c r="C24" s="3">
+        <v>9</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B25" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="2">
-        <f>SUM(C6:C23)</f>
-        <v>98</v>
-      </c>
-      <c r="D24" s="2"/>
+      <c r="C25" s="2">
+        <f>SUM(C6:C24)</f>
+        <v>107</v>
+      </c>
+      <c r="D25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Improved about page. Also started properly work on systeminfromation. Wierd issue being encountered with it have to look into it.
</commit_message>
<xml_diff>
--- a/Material/Työaikaraportti_ArttuMutka.xlsx
+++ b/Material/Työaikaraportti_ArttuMutka.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\School\Ohjelmistokehitys\Project\Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834FD00C-F600-4505-AD12-6065E5C0A210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D3C471-8A90-4F03-ADD2-11377E1A2ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D29C344C-A0B2-4C12-8324-F197E4D0F762}"/>
+    <workbookView xWindow="2220" yWindow="630" windowWidth="21600" windowHeight="11295" xr2:uid="{D29C344C-A0B2-4C12-8324-F197E4D0F762}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Työaikaraportti</t>
   </si>
@@ -110,7 +110,10 @@
     <t>Suunitelin ikonin ja kehitin sen. Tein muunnin työkaluun paranuksia.</t>
   </si>
   <si>
-    <t>Aloin suunitelemaana lisää ominaisuuksia. Implementoin uusia usercontrol ja niille omat navigaatio osiot. Lajitelin tiedostoja paremmin. Tein random number generaatorin. Tein Yksinkertaisen checksum työkalun</t>
+    <t>Paransin about sivua. Myöskin koitin ideoida ja parantaa systeminformation työkalua</t>
+  </si>
+  <si>
+    <t>Aloin suunitelemaana lisää ominaisuuksia. Implementoin uusia usercontrol ja niille omat navigaatio osiot. Lajitelin tiedostoja paremmin. Tein random number generaatorin. Tein Yksinkertaisen checksum työkalun. Aloitin systeminformation.</t>
   </si>
 </sst>
 </file>
@@ -519,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A8DA42-B604-4C4D-9F58-45BF577D224E}">
-  <dimension ref="B2:D25"/>
+  <dimension ref="B2:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,18 +757,29 @@
         <v>9</v>
       </c>
       <c r="D24" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="B25" s="5">
+        <v>45347</v>
+      </c>
+      <c r="C25" s="3">
+        <v>6</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B25" s="2" t="s">
+    <row r="26" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B26" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="2">
-        <f>SUM(C6:C24)</f>
-        <v>107</v>
-      </c>
-      <c r="D25" s="2"/>
+      <c r="C26" s="2">
+        <f>SUM(C6:C25)</f>
+        <v>113</v>
+      </c>
+      <c r="D26" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Made systeminformation tab and tool, still needs some work to be good.
</commit_message>
<xml_diff>
--- a/Material/Työaikaraportti_ArttuMutka.xlsx
+++ b/Material/Työaikaraportti_ArttuMutka.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\School\Ohjelmistokehitys\Project\Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D3C471-8A90-4F03-ADD2-11377E1A2ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F703563-60DE-4991-A6AA-9B8AE7FB2DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2220" yWindow="630" windowWidth="21600" windowHeight="11295" xr2:uid="{D29C344C-A0B2-4C12-8324-F197E4D0F762}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Työaikaraportti</t>
   </si>
@@ -114,6 +114,18 @@
   </si>
   <si>
     <t>Aloin suunitelemaana lisää ominaisuuksia. Implementoin uusia usercontrol ja niille omat navigaatio osiot. Lajitelin tiedostoja paremmin. Tein random number generaatorin. Tein Yksinkertaisen checksum työkalun. Aloitin systeminformation.</t>
+  </si>
+  <si>
+    <t>Katsoin systeminformation työakalua taisin löytää tavan implementoida sen pitää ottaa selvää paremmin</t>
+  </si>
+  <si>
+    <t>Sain systeminformation toimimaan perus tasolla mutta sen pöivityminen ja tyylitely on vielä työn alla</t>
+  </si>
+  <si>
+    <t>Koitin saada systeminformaation päivitämään oikealla tavalla. Sain jotain edistyksiä mutta paljon vaikeuksia saada päivitäminen pyörimään erilisellä thread:lla</t>
+  </si>
+  <si>
+    <t>Kirjoitin dokumentaatiota. Korjasin suurimalta osalta systeminformation vaikkakin vaatii hiomista.</t>
   </si>
 </sst>
 </file>
@@ -522,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A8DA42-B604-4C4D-9F58-45BF577D224E}">
-  <dimension ref="B2:D26"/>
+  <dimension ref="B2:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,7 +774,7 @@
     </row>
     <row r="25" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="B25" s="5">
-        <v>45347</v>
+        <v>45346</v>
       </c>
       <c r="C25" s="3">
         <v>6</v>
@@ -771,15 +783,59 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B26" s="2" t="s">
+    <row r="26" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="B26" s="5">
+        <v>45347</v>
+      </c>
+      <c r="C26" s="3">
         <v>4</v>
       </c>
-      <c r="C26" s="2">
-        <f>SUM(C6:C25)</f>
-        <v>113</v>
-      </c>
-      <c r="D26" s="2"/>
+      <c r="D26" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="B27" s="5">
+        <v>45348</v>
+      </c>
+      <c r="C27" s="3">
+        <v>4</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="B28" s="5">
+        <v>45349</v>
+      </c>
+      <c r="C28" s="3">
+        <v>8</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="B29" s="5">
+        <v>45350</v>
+      </c>
+      <c r="C29" s="3">
+        <v>4</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="2">
+        <f>SUM(C6:C29)</f>
+        <v>133</v>
+      </c>
+      <c r="D30" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Improved responsive and styling of systeminformation
</commit_message>
<xml_diff>
--- a/Material/Työaikaraportti_ArttuMutka.xlsx
+++ b/Material/Työaikaraportti_ArttuMutka.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\School\Ohjelmistokehitys\Project\Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F703563-60DE-4991-A6AA-9B8AE7FB2DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D7DF77-BD87-4E8D-B52E-E200CCCE0E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2220" yWindow="630" windowWidth="21600" windowHeight="11295" xr2:uid="{D29C344C-A0B2-4C12-8324-F197E4D0F762}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Työaikaraportti</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>Kirjoitin dokumentaatiota. Korjasin suurimalta osalta systeminformation vaikkakin vaatii hiomista.</t>
+  </si>
+  <si>
+    <t>Paransin systeminformation tyylitelyä ja lataamista saadakseen käytäjä kokemuksen paremaksi.</t>
   </si>
 </sst>
 </file>
@@ -534,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A8DA42-B604-4C4D-9F58-45BF577D224E}">
-  <dimension ref="B2:D30"/>
+  <dimension ref="B2:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,15 +830,26 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B30" s="2" t="s">
+    <row r="30" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="B30" s="5">
+        <v>45351</v>
+      </c>
+      <c r="C30" s="3">
         <v>4</v>
       </c>
-      <c r="C30" s="2">
-        <f>SUM(C6:C29)</f>
-        <v>133</v>
-      </c>
-      <c r="D30" s="2"/>
+      <c r="D30" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="2">
+        <f>SUM(C6:C30)</f>
+        <v>137</v>
+      </c>
+      <c r="D31" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Made the navigation bar generation be more dynamic and better. Also fixed gitignore file to allow the code to be uploaded to git. Due to modular change to navbar an settings modularity update would be beneficial.
</commit_message>
<xml_diff>
--- a/Material/Työaikaraportti_ArttuMutka.xlsx
+++ b/Material/Työaikaraportti_ArttuMutka.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\School\Ohjelmistokehitys\Project\Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D7DF77-BD87-4E8D-B52E-E200CCCE0E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2A87DF-8627-48E6-A288-B25EB3EA6D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="630" windowWidth="21600" windowHeight="11295" xr2:uid="{D29C344C-A0B2-4C12-8324-F197E4D0F762}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D29C344C-A0B2-4C12-8324-F197E4D0F762}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Työaikaraportti</t>
   </si>
@@ -129,6 +129,18 @@
   </si>
   <si>
     <t>Paransin systeminformation tyylitelyä ja lataamista saadakseen käytäjä kokemuksen paremaksi.</t>
+  </si>
+  <si>
+    <t>Koitin tehdä työkaluista enemmän dynaamisia. Onnistuin ideoimaan hyvän implementointi metodin.</t>
+  </si>
+  <si>
+    <t>Muutin navigaatiopalkin luomisen enemmän moduulariksi. Vaatii vielä vähän hiomista asetusten ja joidenkin tiedostojen suhteen.</t>
+  </si>
+  <si>
+    <t>Koitin saada modulaarisen navigaatiopalkin toimimaan täysin oikein. En saanut yhtä tiedostoa toimimaan oikein.</t>
+  </si>
+  <si>
+    <t>Sain modulaarisen navigaation toimimaan kunolla. Korjasin gitignore</t>
   </si>
 </sst>
 </file>
@@ -537,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A8DA42-B604-4C4D-9F58-45BF577D224E}">
-  <dimension ref="B2:D31"/>
+  <dimension ref="B2:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,21 +847,65 @@
         <v>45351</v>
       </c>
       <c r="C30" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B31" s="2" t="s">
+    <row r="31" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="B31" s="5">
+        <v>45352</v>
+      </c>
+      <c r="C31" s="3">
+        <v>1</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="B32" s="5">
+        <v>45355</v>
+      </c>
+      <c r="C32" s="3">
         <v>4</v>
       </c>
-      <c r="C31" s="2">
-        <f>SUM(C6:C30)</f>
-        <v>137</v>
-      </c>
-      <c r="D31" s="2"/>
+      <c r="D32" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="B33" s="5">
+        <v>45356</v>
+      </c>
+      <c r="C33" s="3">
+        <v>3</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="B34" s="5">
+        <v>45357</v>
+      </c>
+      <c r="C34" s="3">
+        <v>5</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="2">
+        <f>SUM(C6:C34)</f>
+        <v>148</v>
+      </c>
+      <c r="D35" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Made the settings get the defualt page dynamically to ensure proper workinh with multiple files
</commit_message>
<xml_diff>
--- a/Material/Työaikaraportti_ArttuMutka.xlsx
+++ b/Material/Työaikaraportti_ArttuMutka.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\School\Ohjelmistokehitys\Project\Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2A87DF-8627-48E6-A288-B25EB3EA6D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F22D41-8A33-44CB-87D2-F06392D428C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D29C344C-A0B2-4C12-8324-F197E4D0F762}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Työaikaraportti</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>Sain modulaarisen navigaation toimimaan kunolla. Korjasin gitignore</t>
+  </si>
+  <si>
+    <t>Koitin saada asetuksiin liityvät normi sivu toiminnot toimimaan modulaarisesti</t>
+  </si>
+  <si>
+    <t>Sain asetukset toimimaan oikein modulaarisesti normi sivu toiminnon osalta</t>
   </si>
 </sst>
 </file>
@@ -549,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A8DA42-B604-4C4D-9F58-45BF577D224E}">
-  <dimension ref="B2:D35"/>
+  <dimension ref="B2:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,15 +903,37 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B35" s="2" t="s">
+    <row r="35" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="B35" s="5">
+        <v>45358</v>
+      </c>
+      <c r="C35" s="3">
+        <v>2</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="B36" s="5">
+        <v>45359</v>
+      </c>
+      <c r="C36" s="3">
+        <v>5</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B37" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C35" s="2">
-        <f>SUM(C6:C34)</f>
-        <v>148</v>
-      </c>
-      <c r="D35" s="2"/>
+      <c r="C37" s="2">
+        <f>SUM(C6:C36)</f>
+        <v>155</v>
+      </c>
+      <c r="D37" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated materials and dictionary structures.
</commit_message>
<xml_diff>
--- a/Material/Työaikaraportti_ArttuMutka.xlsx
+++ b/Material/Työaikaraportti_ArttuMutka.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\School\Ohjelmistokehitys\Project\Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F22D41-8A33-44CB-87D2-F06392D428C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C567D2EB-F92C-4572-838E-92C1AFAD9A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D29C344C-A0B2-4C12-8324-F197E4D0F762}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Työaikaraportti</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>Sain asetukset toimimaan oikein modulaarisesti normi sivu toiminnon osalta</t>
+  </si>
+  <si>
+    <t>Tein viimeistelyä projektiin sen tiedostoihin ja rakenteeseen ja palautin projektin</t>
   </si>
 </sst>
 </file>
@@ -555,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A8DA42-B604-4C4D-9F58-45BF577D224E}">
-  <dimension ref="B2:D37"/>
+  <dimension ref="B2:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,15 +928,26 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B37" s="2" t="s">
+    <row r="37" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="B37" s="5">
+        <v>45360</v>
+      </c>
+      <c r="C37" s="3">
+        <v>1</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B38" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C37" s="2">
-        <f>SUM(C6:C36)</f>
-        <v>155</v>
-      </c>
-      <c r="D37" s="2"/>
+      <c r="C38" s="2">
+        <f>SUM(C6:C37)</f>
+        <v>156</v>
+      </c>
+      <c r="D38" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>